<commit_message>
New report for TransportVehicleMissions, money for the missions, income of a company, income to the company from the DriverEmployees and change of relationship between client and company - now it is many-to-many.
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/Excel files/output.xlsx
+++ b/src/main/java/org/example/Excel files/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Driver id</t>
   </si>
   <si>
     <t>2023-12-03</t>
@@ -110,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -147,22 +150,25 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>4.0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
         <v>1500.0</v>
@@ -171,13 +177,16 @@
         <v>10.0</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -185,16 +194,16 @@
         <v>5.0</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
         <v>1500.0</v>
@@ -203,13 +212,16 @@
         <v>10.0</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>